<commit_message>
updating with March 2024 invoicing
</commit_message>
<xml_diff>
--- a/ETO Use.xlsx
+++ b/ETO Use.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0450E990-30DC-B642-A786-5A2364071330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF8A3AB-BD9D-7949-BFF9-0FC21BF1F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39980" yWindow="-2180" windowWidth="25760" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="1080" windowWidth="20500" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,45 @@
   </si>
   <si>
     <t>official</t>
+  </si>
+  <si>
+    <t>MRE541</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>emergency medicine</t>
+  </si>
+  <si>
+    <t>radiology</t>
+  </si>
+  <si>
+    <t>cardiology</t>
+  </si>
+  <si>
+    <t>CL013</t>
+  </si>
+  <si>
+    <t>CL011</t>
+  </si>
+  <si>
+    <t>CL012</t>
+  </si>
+  <si>
+    <t>Guillaume Hoareau</t>
+  </si>
+  <si>
+    <t>Improving mitochondrial function to mitigate ischemia-reperfusion injury from aortic occlusion in a swine model of hemorrhagic shock.</t>
+  </si>
+  <si>
+    <t>The mechanisms of GJA1 protection after resuscitation and mitochondrial protection in a pig model of polytrauma</t>
+  </si>
+  <si>
+    <t>Physiologic signatures for endovascular intervention for trauma</t>
+  </si>
+  <si>
+    <t>Silverton/Hoareau</t>
   </si>
 </sst>
 </file>
@@ -538,15 +577,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="2"/>
     <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1317,7 +1356,7 @@
         <v>0.25</v>
       </c>
       <c r="F37">
-        <f t="shared" ref="F37:F51" si="1">E37*40</f>
+        <f t="shared" ref="F37:F56" si="1">E37*40</f>
         <v>10</v>
       </c>
     </row>
@@ -1516,7 +1555,7 @@
         <v>16</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" ref="E48:E51" si="2">1/3</f>
+        <f t="shared" ref="E48:E49" si="2">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="F48">
@@ -1580,6 +1619,84 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" s="2">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>13.333333333333332</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" ref="E54:E55" si="3">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>13.333333333333332</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>13.333333333333332</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1590,20 +1707,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="136" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="136" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1614,10 +1731,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1628,12 +1748,15 @@
         <v>52</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -1642,93 +1765,114 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1737,35 +1881,112 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
streamlining code to require less pre-processing
</commit_message>
<xml_diff>
--- a/ETO Use.xlsx
+++ b/ETO Use.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF8A3AB-BD9D-7949-BFF9-0FC21BF1F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD61B625-3ED3-9644-A316-A36234A2764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1080" windowWidth="20500" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="1080" windowWidth="25020" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
     <sheet name="CL Codes" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="eto_use_alt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,36 @@
   </si>
   <si>
     <t>Silverton/Hoareau</t>
+  </si>
+  <si>
+    <t>CL007, CL002</t>
+  </si>
+  <si>
+    <t>CL003, CL002, CL001, CL007</t>
+  </si>
+  <si>
+    <t>CL002, CL007</t>
+  </si>
+  <si>
+    <t>CL003, CL001, CL007, CL002, CL006</t>
+  </si>
+  <si>
+    <t>CL003, CL006, CL001, CL002</t>
+  </si>
+  <si>
+    <t>CL003, CL001, CL006, CL002</t>
+  </si>
+  <si>
+    <t>CL001, CL004, CL006</t>
+  </si>
+  <si>
+    <t>CL010, CL001, CL000</t>
+  </si>
+  <si>
+    <t>CL010, CL001</t>
+  </si>
+  <si>
+    <t>CL010, CL001, CL013</t>
   </si>
 </sst>
 </file>
@@ -579,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1386,7 @@
         <v>0.25</v>
       </c>
       <c r="F37">
-        <f t="shared" ref="F37:F56" si="1">E37*40</f>
+        <f t="shared" ref="F37:F55" si="1">E37*40</f>
         <v>10</v>
       </c>
     </row>
@@ -1709,7 +1739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1997,12 +2027,237 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44748</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44914</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44971</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45015</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45029</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45062</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45085</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45160</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>45162</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45166</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45194</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45197</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45209</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45225</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>45237</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>45244</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>45293</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>45295</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>45309</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>45328</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>45344</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updating with July charges
</commit_message>
<xml_diff>
--- a/ETO Use.xlsx
+++ b/ETO Use.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE5DBF8-7348-0D41-AFD9-24C367372645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EAE12F-97F2-F140-85BE-746788557626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="2300" windowWidth="25020" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="2300" windowWidth="25020" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -273,6 +273,18 @@
   </si>
   <si>
     <t>CL006, CL007</t>
+  </si>
+  <si>
+    <t>CL015</t>
+  </si>
+  <si>
+    <t>CL015, CL006, CL008</t>
+  </si>
+  <si>
+    <t>Guillaume Hoareau/Austin Johnson</t>
+  </si>
+  <si>
+    <t>Hoareau/Johnson</t>
   </si>
 </sst>
 </file>
@@ -1752,10 +1764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2072,6 +2084,20 @@
         <v>2348</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2080,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2333,6 +2359,30 @@
         <v>80</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>45481</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>45482</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>45490</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updating with august and september charges
</commit_message>
<xml_diff>
--- a/ETO Use.xlsx
+++ b/ETO Use.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EAE12F-97F2-F140-85BE-746788557626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71124AA-C0B6-FD41-8DF5-D5D38E7F18CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="2300" windowWidth="25020" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="2300" windowWidth="25020" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETO Use" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Hoareau/Johnson</t>
+  </si>
+  <si>
+    <t>CL006, CL015</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
@@ -1766,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2106,9 +2109,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -2383,6 +2386,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>45545</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>